<commit_message>
DM themes rough draft
</commit_message>
<xml_diff>
--- a/DataInput/Yan-Zheng-Compustat-Vars.xlsx
+++ b/DataInput/Yan-Zheng-Compustat-Vars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2100f564d45fdb98/AC-RISK-VS/flex-mining/DataInput/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Risk-vs-ac\flex-mining\DataInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="11_046C9CC85795BD032074E768E2BC070891C95D08" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CE8CD3F-B3B2-450D-A016-766FDCFEA4D4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18AB41B-8D4A-46D1-9EA2-A644BD2FAAB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-15" windowWidth="26880" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="633">
   <si>
     <t>id</t>
   </si>
@@ -557,9 +557,6 @@
     <t>Dividends – preferred/preference</t>
   </si>
   <si>
-    <t>Dividends preferred/preference</t>
-  </si>
-  <si>
     <t>DVPA</t>
   </si>
   <si>
@@ -1136,9 +1133,6 @@
     <t>Nonoperating income (expense)</t>
   </si>
   <si>
-    <t>Nonoperating income</t>
-  </si>
-  <si>
     <t>NOPIO</t>
   </si>
   <si>
@@ -1310,9 +1304,6 @@
     <t>Preferred/preference stock (capital) – total</t>
   </si>
   <si>
-    <t>Preferred stock</t>
-  </si>
-  <si>
     <t>PSTKC</t>
   </si>
   <si>
@@ -1331,18 +1322,12 @@
     <t>Preferred/preference stock – nonredeemable</t>
   </si>
   <si>
-    <t>Preferred/preference stock nonredeemable</t>
-  </si>
-  <si>
     <t>PSTKR</t>
   </si>
   <si>
     <t>Preferred/preference stock – redeemable</t>
   </si>
   <si>
-    <t>Preferred/preference stock redeemable</t>
-  </si>
-  <si>
     <t>PSTKRV</t>
   </si>
   <si>
@@ -1908,6 +1893,45 @@
   </si>
   <si>
     <t>Deferred taxes cash flow</t>
+  </si>
+  <si>
+    <t>Pref stock</t>
+  </si>
+  <si>
+    <t>Pref stock convertible</t>
+  </si>
+  <si>
+    <t>Pref stock nonredeemable</t>
+  </si>
+  <si>
+    <t>Pref stock redeemable</t>
+  </si>
+  <si>
+    <t>Pref stock liq value</t>
+  </si>
+  <si>
+    <t>Cap surplus reserve</t>
+  </si>
+  <si>
+    <t>Notes payable st</t>
+  </si>
+  <si>
+    <t>Nonop income</t>
+  </si>
+  <si>
+    <t>Nonop income other</t>
+  </si>
+  <si>
+    <t>Dividends common</t>
+  </si>
+  <si>
+    <t>Dividends pref</t>
+  </si>
+  <si>
+    <t>Income bef extraord</t>
+  </si>
+  <si>
+    <t>Def taxes + inv tax cred</t>
   </si>
 </sst>
 </file>
@@ -2009,10 +2033,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2306,10 +2326,10 @@
   <dimension ref="A1:G243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B189" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B185" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D208" sqref="D208"/>
+      <selection pane="bottomRight" activeCell="D212" sqref="D212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2339,10 +2359,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="G1" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2671,11 +2691,11 @@
         <v>44</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>44</v>
+        <v>625</v>
       </c>
       <c r="E17" s="6">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -2818,7 +2838,7 @@
         <v>61</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="E24" s="6">
         <f t="shared" si="0"/>
@@ -3385,7 +3405,7 @@
         <v>123</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="E51" s="6">
         <f t="shared" si="0"/>
@@ -3637,7 +3657,7 @@
         <v>150</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="E63" s="6">
         <f t="shared" si="0"/>
@@ -3658,7 +3678,7 @@
         <v>152</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="E64" s="6">
         <f t="shared" si="0"/>
@@ -3679,7 +3699,7 @@
         <v>154</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="E65" s="6">
         <f t="shared" si="0"/>
@@ -3826,11 +3846,11 @@
         <v>171</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>171</v>
+        <v>629</v>
       </c>
       <c r="E72" s="6">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F72">
         <v>1</v>
@@ -3847,11 +3867,11 @@
         <v>173</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>174</v>
+        <v>630</v>
       </c>
       <c r="E73" s="6">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="F73">
         <v>1</v>
@@ -3862,13 +3882,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C74" s="2" t="s">
-        <v>176</v>
-      </c>
       <c r="D74" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E74" s="6">
         <f t="shared" si="1"/>
@@ -3883,13 +3903,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="D75" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>179</v>
       </c>
       <c r="E75" s="6">
         <f t="shared" si="1"/>
@@ -3904,13 +3924,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="D76" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="E76" s="6">
         <f t="shared" si="1"/>
@@ -3925,13 +3945,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C77" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C77" s="2" t="s">
-        <v>184</v>
-      </c>
       <c r="D77" s="3" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="E77" s="6">
         <f t="shared" si="1"/>
@@ -3946,13 +3966,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C78" s="2" t="s">
-        <v>186</v>
-      </c>
       <c r="D78" s="3" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="E78" s="6">
         <f t="shared" si="1"/>
@@ -3967,13 +3987,13 @@
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>188</v>
-      </c>
       <c r="D79" s="3" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="E79" s="6">
         <f t="shared" si="1"/>
@@ -3988,13 +4008,13 @@
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C80" s="2" t="s">
-        <v>190</v>
-      </c>
       <c r="D80" s="3" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="E80" s="6">
         <f t="shared" si="1"/>
@@ -4009,13 +4029,13 @@
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C81" s="2" t="s">
-        <v>192</v>
-      </c>
       <c r="D81" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E81" s="6">
         <f t="shared" si="1"/>
@@ -4030,13 +4050,13 @@
         <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>194</v>
-      </c>
       <c r="D82" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E82" s="6">
         <f t="shared" si="1"/>
@@ -4051,13 +4071,13 @@
         <v>82</v>
       </c>
       <c r="B83" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="D83" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>200</v>
       </c>
       <c r="E83" s="6">
         <f t="shared" si="1"/>
@@ -4072,13 +4092,13 @@
         <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="D84" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>203</v>
       </c>
       <c r="E84" s="6">
         <f t="shared" si="1"/>
@@ -4093,13 +4113,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="D85" s="3" t="s">
         <v>205</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>206</v>
       </c>
       <c r="E85" s="6">
         <f t="shared" si="1"/>
@@ -4114,13 +4134,13 @@
         <v>85</v>
       </c>
       <c r="B86" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C86" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="D86" s="3" t="s">
         <v>208</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>209</v>
       </c>
       <c r="E86" s="6">
         <f t="shared" si="1"/>
@@ -4135,13 +4155,13 @@
         <v>86</v>
       </c>
       <c r="B87" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C87" s="2" t="s">
-        <v>211</v>
-      </c>
       <c r="D87" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E87" s="6">
         <f t="shared" si="1"/>
@@ -4156,13 +4176,13 @@
         <v>87</v>
       </c>
       <c r="B88" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C88" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="C88" s="2" t="s">
-        <v>213</v>
-      </c>
       <c r="D88" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E88" s="6">
         <f t="shared" si="1"/>
@@ -4177,13 +4197,13 @@
         <v>88</v>
       </c>
       <c r="B89" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C89" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="D89" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>216</v>
       </c>
       <c r="E89" s="6">
         <f t="shared" si="1"/>
@@ -4198,13 +4218,13 @@
         <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C90" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="D90" s="3" t="s">
         <v>218</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>219</v>
       </c>
       <c r="E90" s="6">
         <f t="shared" si="1"/>
@@ -4219,13 +4239,13 @@
         <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="D91" s="3" t="s">
         <v>221</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>222</v>
       </c>
       <c r="E91" s="6">
         <f t="shared" si="1"/>
@@ -4240,13 +4260,13 @@
         <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="D92" s="3" t="s">
         <v>224</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>225</v>
       </c>
       <c r="E92" s="6">
         <f t="shared" si="1"/>
@@ -4261,13 +4281,13 @@
         <v>92</v>
       </c>
       <c r="B93" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C93" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="D93" s="3" t="s">
         <v>227</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>228</v>
       </c>
       <c r="E93" s="6">
         <f t="shared" si="1"/>
@@ -4282,13 +4302,13 @@
         <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="D94" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="E94" s="6">
         <f t="shared" si="1"/>
@@ -4303,13 +4323,13 @@
         <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="D95" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>234</v>
       </c>
       <c r="E95" s="6">
         <f t="shared" si="1"/>
@@ -4324,13 +4344,13 @@
         <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C96" s="2" t="s">
-        <v>236</v>
-      </c>
       <c r="D96" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E96" s="6">
         <f t="shared" si="1"/>
@@ -4345,13 +4365,13 @@
         <v>96</v>
       </c>
       <c r="B97" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C97" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C97" s="2" t="s">
-        <v>238</v>
-      </c>
       <c r="D97" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E97" s="6">
         <f t="shared" si="1"/>
@@ -4366,13 +4386,13 @@
         <v>97</v>
       </c>
       <c r="B98" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C98" s="2" t="s">
-        <v>240</v>
-      </c>
       <c r="D98" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E98" s="6">
         <f t="shared" si="1"/>
@@ -4387,13 +4407,13 @@
         <v>98</v>
       </c>
       <c r="B99" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C99" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="D99" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>243</v>
       </c>
       <c r="E99" s="6">
         <f t="shared" si="1"/>
@@ -4408,13 +4428,13 @@
         <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C100" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C100" s="2" t="s">
-        <v>245</v>
-      </c>
       <c r="D100" s="3" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="E100" s="6">
         <f t="shared" si="1"/>
@@ -4429,13 +4449,13 @@
         <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C101" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="C101" s="2" t="s">
-        <v>247</v>
-      </c>
       <c r="D101" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E101" s="6">
         <f t="shared" si="1"/>
@@ -4450,13 +4470,13 @@
         <v>101</v>
       </c>
       <c r="B102" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C102" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C102" s="2" t="s">
-        <v>249</v>
-      </c>
       <c r="D102" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E102" s="6">
         <f t="shared" si="1"/>
@@ -4471,13 +4491,13 @@
         <v>102</v>
       </c>
       <c r="B103" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C103" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="C103" s="2" t="s">
-        <v>251</v>
-      </c>
       <c r="D103" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E103" s="6">
         <f t="shared" si="1"/>
@@ -4492,13 +4512,13 @@
         <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C104" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="C104" s="2" t="s">
-        <v>253</v>
-      </c>
       <c r="D104" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E104" s="6">
         <f t="shared" si="1"/>
@@ -4513,13 +4533,13 @@
         <v>104</v>
       </c>
       <c r="B105" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="C105" s="2" t="s">
-        <v>255</v>
-      </c>
       <c r="D105" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E105" s="6">
         <f t="shared" si="1"/>
@@ -4534,13 +4554,13 @@
         <v>105</v>
       </c>
       <c r="B106" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C106" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="D106" s="3" t="s">
         <v>257</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>258</v>
       </c>
       <c r="E106" s="6">
         <f t="shared" si="1"/>
@@ -4555,17 +4575,17 @@
         <v>106</v>
       </c>
       <c r="B107" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C107" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="C107" s="2" t="s">
-        <v>260</v>
-      </c>
       <c r="D107" s="3" t="s">
-        <v>260</v>
+        <v>631</v>
       </c>
       <c r="E107" s="6">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="F107">
         <v>1</v>
@@ -4576,13 +4596,13 @@
         <v>107</v>
       </c>
       <c r="B108" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C108" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C108" s="2" t="s">
-        <v>262</v>
-      </c>
       <c r="D108" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E108" s="6">
         <f t="shared" si="1"/>
@@ -4597,13 +4617,13 @@
         <v>108</v>
       </c>
       <c r="B109" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C109" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C109" s="2" t="s">
-        <v>264</v>
-      </c>
       <c r="D109" s="3" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="E109" s="6">
         <f t="shared" si="1"/>
@@ -4618,13 +4638,13 @@
         <v>109</v>
       </c>
       <c r="B110" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C110" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C110" s="2" t="s">
+      <c r="D110" s="3" t="s">
         <v>266</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>267</v>
       </c>
       <c r="E110" s="6">
         <f t="shared" si="1"/>
@@ -4639,13 +4659,13 @@
         <v>110</v>
       </c>
       <c r="B111" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C111" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="D111" s="3" t="s">
         <v>269</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>270</v>
       </c>
       <c r="E111" s="6">
         <f t="shared" si="1"/>
@@ -4660,13 +4680,13 @@
         <v>111</v>
       </c>
       <c r="B112" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C112" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="D112" s="3" t="s">
         <v>272</v>
-      </c>
-      <c r="D112" s="3" t="s">
-        <v>273</v>
       </c>
       <c r="E112" s="6">
         <f t="shared" si="1"/>
@@ -4681,13 +4701,13 @@
         <v>112</v>
       </c>
       <c r="B113" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C113" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="D113" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>276</v>
       </c>
       <c r="E113" s="6">
         <f t="shared" si="1"/>
@@ -4702,13 +4722,13 @@
         <v>113</v>
       </c>
       <c r="B114" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C114" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C114" s="2" t="s">
-        <v>278</v>
-      </c>
       <c r="D114" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E114" s="6">
         <f t="shared" si="1"/>
@@ -4723,13 +4743,13 @@
         <v>114</v>
       </c>
       <c r="B115" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C115" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="C115" s="2" t="s">
-        <v>280</v>
-      </c>
       <c r="D115" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E115" s="6">
         <f t="shared" si="1"/>
@@ -4744,13 +4764,13 @@
         <v>115</v>
       </c>
       <c r="B116" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C116" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="D116" s="3" t="s">
         <v>282</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>283</v>
       </c>
       <c r="E116" s="6">
         <f t="shared" si="1"/>
@@ -4765,13 +4785,13 @@
         <v>116</v>
       </c>
       <c r="B117" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C117" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C117" s="2" t="s">
-        <v>285</v>
-      </c>
       <c r="D117" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E117" s="6">
         <f t="shared" si="1"/>
@@ -4786,13 +4806,13 @@
         <v>117</v>
       </c>
       <c r="B118" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C118" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="C118" s="2" t="s">
-        <v>287</v>
-      </c>
       <c r="D118" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E118" s="6">
         <f t="shared" si="1"/>
@@ -4807,13 +4827,13 @@
         <v>118</v>
       </c>
       <c r="B119" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C119" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C119" s="2" t="s">
-        <v>289</v>
-      </c>
       <c r="D119" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E119" s="6">
         <f t="shared" si="1"/>
@@ -4828,13 +4848,13 @@
         <v>119</v>
       </c>
       <c r="B120" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C120" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="D120" s="3" t="s">
         <v>291</v>
-      </c>
-      <c r="D120" s="3" t="s">
-        <v>292</v>
       </c>
       <c r="E120" s="6">
         <f t="shared" si="1"/>
@@ -4849,13 +4869,13 @@
         <v>120</v>
       </c>
       <c r="B121" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C121" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C121" s="2" t="s">
-        <v>294</v>
-      </c>
       <c r="D121" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E121" s="6">
         <f t="shared" si="1"/>
@@ -4870,13 +4890,13 @@
         <v>121</v>
       </c>
       <c r="B122" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C122" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="D122" s="3" t="s">
         <v>296</v>
-      </c>
-      <c r="D122" s="3" t="s">
-        <v>297</v>
       </c>
       <c r="E122" s="6">
         <f t="shared" si="1"/>
@@ -4891,13 +4911,13 @@
         <v>122</v>
       </c>
       <c r="B123" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C123" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C123" s="2" t="s">
+      <c r="D123" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="D123" s="3" t="s">
-        <v>300</v>
       </c>
       <c r="E123" s="6">
         <f t="shared" si="1"/>
@@ -4912,13 +4932,13 @@
         <v>123</v>
       </c>
       <c r="B124" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C124" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C124" s="2" t="s">
-        <v>302</v>
-      </c>
       <c r="D124" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E124" s="6">
         <f t="shared" si="1"/>
@@ -4933,13 +4953,13 @@
         <v>124</v>
       </c>
       <c r="B125" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C125" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="C125" s="2" t="s">
+      <c r="D125" s="3" t="s">
         <v>304</v>
-      </c>
-      <c r="D125" s="3" t="s">
-        <v>305</v>
       </c>
       <c r="E125" s="6">
         <f t="shared" si="1"/>
@@ -4954,13 +4974,13 @@
         <v>125</v>
       </c>
       <c r="B126" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C126" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="C126" s="2" t="s">
+      <c r="D126" s="3" t="s">
         <v>307</v>
-      </c>
-      <c r="D126" s="3" t="s">
-        <v>308</v>
       </c>
       <c r="E126" s="6">
         <f t="shared" si="1"/>
@@ -4975,13 +4995,13 @@
         <v>126</v>
       </c>
       <c r="B127" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C127" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="C127" s="2" t="s">
-        <v>310</v>
-      </c>
       <c r="D127" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E127" s="6">
         <f t="shared" si="1"/>
@@ -4996,13 +5016,13 @@
         <v>127</v>
       </c>
       <c r="B128" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C128" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="C128" s="2" t="s">
-        <v>312</v>
-      </c>
       <c r="D128" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E128" s="6">
         <f t="shared" si="1"/>
@@ -5017,13 +5037,13 @@
         <v>128</v>
       </c>
       <c r="B129" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C129" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="D129" s="3" t="s">
         <v>314</v>
-      </c>
-      <c r="D129" s="3" t="s">
-        <v>315</v>
       </c>
       <c r="E129" s="6">
         <f t="shared" si="1"/>
@@ -5038,13 +5058,13 @@
         <v>129</v>
       </c>
       <c r="B130" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C130" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C130" s="2" t="s">
+      <c r="D130" s="3" t="s">
         <v>317</v>
-      </c>
-      <c r="D130" s="3" t="s">
-        <v>318</v>
       </c>
       <c r="E130" s="6">
         <f t="shared" ref="E130:E193" si="2">LEN(D130)</f>
@@ -5059,13 +5079,13 @@
         <v>130</v>
       </c>
       <c r="B131" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C131" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="C131" s="2" t="s">
-        <v>320</v>
-      </c>
       <c r="D131" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E131" s="6">
         <f t="shared" si="2"/>
@@ -5080,13 +5100,13 @@
         <v>131</v>
       </c>
       <c r="B132" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C132" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="C132" s="2" t="s">
-        <v>322</v>
-      </c>
       <c r="D132" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E132" s="6">
         <f t="shared" si="2"/>
@@ -5101,13 +5121,13 @@
         <v>132</v>
       </c>
       <c r="B133" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C133" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C133" s="2" t="s">
-        <v>324</v>
-      </c>
       <c r="D133" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E133" s="6">
         <f t="shared" si="2"/>
@@ -5122,13 +5142,13 @@
         <v>133</v>
       </c>
       <c r="B134" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C134" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="C134" s="2" t="s">
+      <c r="D134" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>327</v>
       </c>
       <c r="E134" s="6">
         <f t="shared" si="2"/>
@@ -5143,13 +5163,13 @@
         <v>134</v>
       </c>
       <c r="B135" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C135" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="C135" s="2" t="s">
-        <v>329</v>
-      </c>
       <c r="D135" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E135" s="6">
         <f t="shared" si="2"/>
@@ -5164,13 +5184,13 @@
         <v>135</v>
       </c>
       <c r="B136" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C136" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="C136" s="2" t="s">
+      <c r="D136" s="3" t="s">
         <v>331</v>
-      </c>
-      <c r="D136" s="3" t="s">
-        <v>332</v>
       </c>
       <c r="E136" s="6">
         <f t="shared" si="2"/>
@@ -5185,13 +5205,13 @@
         <v>136</v>
       </c>
       <c r="B137" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C137" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="C137" s="2" t="s">
+      <c r="D137" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="D137" s="3" t="s">
-        <v>335</v>
       </c>
       <c r="E137" s="6">
         <f t="shared" si="2"/>
@@ -5206,13 +5226,13 @@
         <v>137</v>
       </c>
       <c r="B138" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C138" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C138" s="2" t="s">
+      <c r="D138" s="3" t="s">
         <v>340</v>
-      </c>
-      <c r="D138" s="3" t="s">
-        <v>341</v>
       </c>
       <c r="E138" s="6">
         <f t="shared" si="2"/>
@@ -5227,13 +5247,13 @@
         <v>138</v>
       </c>
       <c r="B139" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C139" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="C139" s="2" t="s">
-        <v>343</v>
-      </c>
       <c r="D139" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E139" s="6">
         <f t="shared" si="2"/>
@@ -5248,13 +5268,13 @@
         <v>139</v>
       </c>
       <c r="B140" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C140" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="C140" s="2" t="s">
-        <v>345</v>
-      </c>
       <c r="D140" s="3" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="E140" s="6">
         <f t="shared" si="2"/>
@@ -5269,13 +5289,13 @@
         <v>140</v>
       </c>
       <c r="B141" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="C141" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="C141" s="2" t="s">
-        <v>347</v>
-      </c>
       <c r="D141" s="3" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="E141" s="6">
         <f t="shared" si="2"/>
@@ -5290,13 +5310,13 @@
         <v>141</v>
       </c>
       <c r="B142" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C142" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="C142" s="2" t="s">
-        <v>349</v>
-      </c>
       <c r="D142" s="3" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="E142" s="6">
         <f t="shared" si="2"/>
@@ -5311,13 +5331,13 @@
         <v>142</v>
       </c>
       <c r="B143" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C143" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="C143" s="2" t="s">
-        <v>351</v>
-      </c>
       <c r="D143" s="3" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="E143" s="6">
         <f t="shared" si="2"/>
@@ -5332,13 +5352,13 @@
         <v>143</v>
       </c>
       <c r="B144" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C144" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="C144" s="2" t="s">
-        <v>353</v>
-      </c>
       <c r="D144" s="3" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="E144" s="6">
         <f t="shared" si="2"/>
@@ -5353,13 +5373,13 @@
         <v>144</v>
       </c>
       <c r="B145" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C145" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="C145" s="2" t="s">
-        <v>355</v>
-      </c>
       <c r="D145" s="3" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="E145" s="6">
         <f t="shared" si="2"/>
@@ -5374,13 +5394,13 @@
         <v>145</v>
       </c>
       <c r="B146" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C146" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="C146" s="2" t="s">
-        <v>357</v>
-      </c>
       <c r="D146" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E146" s="6">
         <f t="shared" si="2"/>
@@ -5395,13 +5415,13 @@
         <v>146</v>
       </c>
       <c r="B147" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C147" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="C147" s="2" t="s">
+      <c r="D147" s="3" t="s">
         <v>359</v>
-      </c>
-      <c r="D147" s="3" t="s">
-        <v>360</v>
       </c>
       <c r="E147" s="6">
         <f t="shared" si="2"/>
@@ -5416,13 +5436,13 @@
         <v>147</v>
       </c>
       <c r="B148" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C148" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="C148" s="2" t="s">
-        <v>362</v>
-      </c>
       <c r="D148" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E148" s="6">
         <f t="shared" si="2"/>
@@ -5437,13 +5457,13 @@
         <v>148</v>
       </c>
       <c r="B149" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C149" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="C149" s="2" t="s">
-        <v>364</v>
-      </c>
       <c r="D149" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E149" s="6">
         <f t="shared" si="2"/>
@@ -5458,17 +5478,17 @@
         <v>149</v>
       </c>
       <c r="B150" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C150" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="C150" s="2" t="s">
-        <v>366</v>
-      </c>
       <c r="D150" s="3" t="s">
-        <v>367</v>
+        <v>627</v>
       </c>
       <c r="E150" s="6">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F150">
         <v>1</v>
@@ -5479,17 +5499,17 @@
         <v>150</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>369</v>
+        <v>628</v>
       </c>
       <c r="E151" s="6">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="F151">
         <v>1</v>
@@ -5500,17 +5520,17 @@
         <v>151</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>371</v>
+        <v>626</v>
       </c>
       <c r="E152" s="6">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="F152">
         <v>1</v>
@@ -5521,13 +5541,13 @@
         <v>152</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E153" s="6">
         <f t="shared" si="2"/>
@@ -5542,13 +5562,13 @@
         <v>153</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E154" s="6">
         <f t="shared" si="2"/>
@@ -5563,13 +5583,13 @@
         <v>154</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="E155" s="6">
         <f t="shared" si="2"/>
@@ -5584,13 +5604,13 @@
         <v>155</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E156" s="6">
         <f t="shared" si="2"/>
@@ -5605,13 +5625,13 @@
         <v>156</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E157" s="6">
         <f t="shared" si="2"/>
@@ -5626,13 +5646,13 @@
         <v>157</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E158" s="6">
         <f t="shared" si="2"/>
@@ -5647,13 +5667,13 @@
         <v>158</v>
       </c>
       <c r="B159" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="D159" s="3" t="s">
         <v>384</v>
-      </c>
-      <c r="C159" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="D159" s="3" t="s">
-        <v>386</v>
       </c>
       <c r="E159" s="6">
         <f t="shared" si="2"/>
@@ -5668,13 +5688,13 @@
         <v>159</v>
       </c>
       <c r="B160" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D160" s="3" t="s">
         <v>387</v>
-      </c>
-      <c r="C160" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="D160" s="3" t="s">
-        <v>389</v>
       </c>
       <c r="E160" s="6">
         <f t="shared" si="2"/>
@@ -5689,13 +5709,13 @@
         <v>160</v>
       </c>
       <c r="B161" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="D161" s="3" t="s">
         <v>390</v>
-      </c>
-      <c r="C161" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D161" s="3" t="s">
-        <v>392</v>
       </c>
       <c r="E161" s="6">
         <f t="shared" si="2"/>
@@ -5710,13 +5730,13 @@
         <v>161</v>
       </c>
       <c r="B162" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="D162" s="3" t="s">
         <v>393</v>
-      </c>
-      <c r="C162" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D162" s="3" t="s">
-        <v>395</v>
       </c>
       <c r="E162" s="6">
         <f t="shared" si="2"/>
@@ -5731,13 +5751,13 @@
         <v>162</v>
       </c>
       <c r="B163" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D163" s="3" t="s">
         <v>396</v>
-      </c>
-      <c r="C163" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="D163" s="3" t="s">
-        <v>398</v>
       </c>
       <c r="E163" s="6">
         <f t="shared" si="2"/>
@@ -5752,13 +5772,13 @@
         <v>163</v>
       </c>
       <c r="B164" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="D164" s="3" t="s">
         <v>399</v>
-      </c>
-      <c r="C164" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="D164" s="3" t="s">
-        <v>401</v>
       </c>
       <c r="E164" s="6">
         <f t="shared" si="2"/>
@@ -5773,13 +5793,13 @@
         <v>164</v>
       </c>
       <c r="B165" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="D165" s="3" t="s">
         <v>402</v>
-      </c>
-      <c r="C165" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="D165" s="3" t="s">
-        <v>404</v>
       </c>
       <c r="E165" s="6">
         <f t="shared" si="2"/>
@@ -5794,13 +5814,13 @@
         <v>165</v>
       </c>
       <c r="B166" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D166" s="3" t="s">
         <v>405</v>
-      </c>
-      <c r="C166" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="D166" s="3" t="s">
-        <v>407</v>
       </c>
       <c r="E166" s="6">
         <f t="shared" si="2"/>
@@ -5815,13 +5835,13 @@
         <v>166</v>
       </c>
       <c r="B167" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D167" s="3" t="s">
         <v>408</v>
-      </c>
-      <c r="C167" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="D167" s="3" t="s">
-        <v>410</v>
       </c>
       <c r="E167" s="6">
         <f t="shared" si="2"/>
@@ -5836,13 +5856,13 @@
         <v>167</v>
       </c>
       <c r="B168" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="D168" s="3" t="s">
         <v>411</v>
-      </c>
-      <c r="C168" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="D168" s="3" t="s">
-        <v>413</v>
       </c>
       <c r="E168" s="6">
         <f t="shared" si="2"/>
@@ -5857,13 +5877,13 @@
         <v>168</v>
       </c>
       <c r="B169" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="D169" s="3" t="s">
         <v>414</v>
-      </c>
-      <c r="C169" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="D169" s="3" t="s">
-        <v>416</v>
       </c>
       <c r="E169" s="6">
         <f t="shared" si="2"/>
@@ -5878,13 +5898,13 @@
         <v>169</v>
       </c>
       <c r="B170" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D170" s="3" t="s">
         <v>417</v>
-      </c>
-      <c r="C170" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D170" s="3" t="s">
-        <v>419</v>
       </c>
       <c r="E170" s="6">
         <f t="shared" si="2"/>
@@ -5899,13 +5919,13 @@
         <v>170</v>
       </c>
       <c r="B171" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="D171" s="3" t="s">
         <v>420</v>
-      </c>
-      <c r="C171" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="D171" s="3" t="s">
-        <v>422</v>
       </c>
       <c r="E171" s="6">
         <f t="shared" si="2"/>
@@ -5920,17 +5940,17 @@
         <v>171</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>425</v>
+        <v>620</v>
       </c>
       <c r="E172" s="6">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F172">
         <v>1</v>
@@ -5941,17 +5961,17 @@
         <v>172</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>427</v>
+        <v>621</v>
       </c>
       <c r="E173" s="6">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F173">
         <v>1</v>
@@ -5962,17 +5982,17 @@
         <v>173</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>429</v>
+        <v>624</v>
       </c>
       <c r="E174" s="6">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="F174">
         <v>1</v>
@@ -5983,17 +6003,17 @@
         <v>174</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>432</v>
+        <v>622</v>
       </c>
       <c r="E175" s="6">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="F175">
         <v>1</v>
@@ -6004,17 +6024,17 @@
         <v>175</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>435</v>
+        <v>623</v>
       </c>
       <c r="E176" s="6">
         <f t="shared" si="2"/>
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="F176">
         <v>1</v>
@@ -6025,13 +6045,13 @@
         <v>176</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="E177" s="6">
         <f t="shared" si="2"/>
@@ -6046,13 +6066,13 @@
         <v>177</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="E178" s="6">
         <f t="shared" si="2"/>
@@ -6067,13 +6087,13 @@
         <v>178</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="E179" s="6">
         <f t="shared" si="2"/>
@@ -6088,13 +6108,13 @@
         <v>179</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="E180" s="6">
         <f t="shared" si="2"/>
@@ -6109,13 +6129,13 @@
         <v>180</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="E181" s="6">
         <f t="shared" si="2"/>
@@ -6130,13 +6150,13 @@
         <v>181</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="E182" s="6">
         <f t="shared" si="2"/>
@@ -6151,13 +6171,13 @@
         <v>182</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="E183" s="6">
         <f t="shared" si="2"/>
@@ -6172,13 +6192,13 @@
         <v>183</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="E184" s="6">
         <f t="shared" si="2"/>
@@ -6193,13 +6213,13 @@
         <v>184</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="E185" s="6">
         <f t="shared" si="2"/>
@@ -6214,13 +6234,13 @@
         <v>185</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="E186" s="6">
         <f t="shared" si="2"/>
@@ -6235,13 +6255,13 @@
         <v>186</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="E187" s="6">
         <f t="shared" si="2"/>
@@ -6256,13 +6276,13 @@
         <v>187</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="E188" s="6">
         <f t="shared" si="2"/>
@@ -6277,13 +6297,13 @@
         <v>188</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="E189" s="6">
         <f t="shared" si="2"/>
@@ -6298,13 +6318,13 @@
         <v>189</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="E190" s="6">
         <f t="shared" si="2"/>
@@ -6319,13 +6339,13 @@
         <v>190</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="E191" s="6">
         <f t="shared" si="2"/>
@@ -6340,13 +6360,13 @@
         <v>191</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="E192" s="6">
         <f t="shared" si="2"/>
@@ -6361,13 +6381,13 @@
         <v>192</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="E193" s="6">
         <f t="shared" si="2"/>
@@ -6382,13 +6402,13 @@
         <v>193</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="E194" s="6">
         <f t="shared" ref="E194:E243" si="3">LEN(D194)</f>
@@ -6403,13 +6423,13 @@
         <v>194</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="E195" s="6">
         <f t="shared" si="3"/>
@@ -6424,13 +6444,13 @@
         <v>195</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="E196" s="6">
         <f t="shared" si="3"/>
@@ -6445,13 +6465,13 @@
         <v>196</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="E197" s="6">
         <f t="shared" si="3"/>
@@ -6466,13 +6486,13 @@
         <v>197</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="E198" s="6">
         <f t="shared" si="3"/>
@@ -6487,13 +6507,13 @@
         <v>198</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="D199" s="3" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="E199" s="6">
         <f t="shared" si="3"/>
@@ -6508,13 +6528,13 @@
         <v>199</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="E200" s="6">
         <f t="shared" si="3"/>
@@ -6529,13 +6549,13 @@
         <v>200</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="E201" s="6">
         <f t="shared" si="3"/>
@@ -6550,13 +6570,13 @@
         <v>201</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="E202" s="6">
         <f t="shared" si="3"/>
@@ -6571,13 +6591,13 @@
         <v>202</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="E203" s="6">
         <f t="shared" si="3"/>
@@ -6592,13 +6612,13 @@
         <v>203</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="E204" s="6">
         <f t="shared" si="3"/>
@@ -6613,13 +6633,13 @@
         <v>204</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="E205" s="6">
         <f t="shared" si="3"/>
@@ -6634,13 +6654,13 @@
         <v>205</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="E206" s="6">
         <f t="shared" si="3"/>
@@ -6655,13 +6675,13 @@
         <v>206</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="E207" s="6">
         <f t="shared" si="3"/>
@@ -6676,13 +6696,13 @@
         <v>207</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="E208" s="6">
         <f t="shared" si="3"/>
@@ -6697,13 +6717,13 @@
         <v>208</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="E209" s="6">
         <f t="shared" si="3"/>
@@ -6718,13 +6738,13 @@
         <v>209</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="E210" s="6">
         <f t="shared" si="3"/>
@@ -6739,17 +6759,17 @@
         <v>210</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>530</v>
+        <v>632</v>
       </c>
       <c r="E211" s="6">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="F211">
         <v>1</v>
@@ -6760,13 +6780,13 @@
         <v>211</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="E212" s="6">
         <f t="shared" si="3"/>
@@ -6781,13 +6801,13 @@
         <v>212</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="E213" s="6">
         <f t="shared" si="3"/>
@@ -6802,13 +6822,13 @@
         <v>213</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="E214" s="6">
         <f t="shared" si="3"/>
@@ -6823,13 +6843,13 @@
         <v>214</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="E215" s="6">
         <f t="shared" si="3"/>
@@ -6844,13 +6864,13 @@
         <v>215</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="D216" s="3" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="E216" s="6">
         <f t="shared" si="3"/>
@@ -6865,13 +6885,13 @@
         <v>216</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="C217" s="3" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="E217" s="6">
         <f t="shared" si="3"/>
@@ -6886,13 +6906,13 @@
         <v>217</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="E218" s="6">
         <f t="shared" si="3"/>
@@ -6907,13 +6927,13 @@
         <v>218</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="E219" s="6">
         <f t="shared" si="3"/>
@@ -6928,13 +6948,13 @@
         <v>219</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="E220" s="6">
         <f t="shared" si="3"/>
@@ -6949,13 +6969,13 @@
         <v>220</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="E221" s="6">
         <f t="shared" si="3"/>
@@ -6970,13 +6990,13 @@
         <v>221</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="E222" s="6">
         <f t="shared" si="3"/>
@@ -6991,13 +7011,13 @@
         <v>222</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="E223" s="6">
         <f t="shared" si="3"/>
@@ -7012,13 +7032,13 @@
         <v>223</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="E224" s="6">
         <f t="shared" si="3"/>
@@ -7033,13 +7053,13 @@
         <v>224</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="D225" s="3" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="E225" s="6">
         <f t="shared" si="3"/>
@@ -7054,13 +7074,13 @@
         <v>225</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="E226" s="6">
         <f t="shared" si="3"/>
@@ -7075,13 +7095,13 @@
         <v>226</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="E227" s="6">
         <f t="shared" si="3"/>
@@ -7096,13 +7116,13 @@
         <v>227</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="E228" s="6">
         <f t="shared" si="3"/>
@@ -7117,13 +7137,13 @@
         <v>228</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="D229" s="3" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="E229" s="6">
         <f t="shared" si="3"/>
@@ -7138,13 +7158,13 @@
         <v>229</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="D230" s="3" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="E230" s="6">
         <f t="shared" si="3"/>
@@ -7159,13 +7179,13 @@
         <v>230</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="D231" s="3" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="E231" s="6">
         <f t="shared" si="3"/>
@@ -7180,13 +7200,13 @@
         <v>231</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="D232" s="3" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="E232" s="6">
         <f t="shared" si="3"/>
@@ -7201,13 +7221,13 @@
         <v>232</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="D233" s="3" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="E233" s="6">
         <f t="shared" si="3"/>
@@ -7222,13 +7242,13 @@
         <v>233</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="C234" s="2" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="D234" s="3" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="E234" s="6">
         <f t="shared" si="3"/>
@@ -7243,13 +7263,13 @@
         <v>234</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="D235" s="3" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="E235" s="6">
         <f t="shared" si="3"/>
@@ -7264,13 +7284,13 @@
         <v>235</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="D236" s="3" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="E236" s="6">
         <f t="shared" si="3"/>
@@ -7285,13 +7305,13 @@
         <v>236</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="D237" s="3" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="E237" s="6">
         <f t="shared" si="3"/>
@@ -7306,13 +7326,13 @@
         <v>237</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="D238" s="3" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="E238" s="6">
         <f t="shared" si="3"/>
@@ -7327,13 +7347,13 @@
         <v>238</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="D239" s="3" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="E239" s="6">
         <f t="shared" si="3"/>
@@ -7348,13 +7368,13 @@
         <v>239</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="D240" s="3" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="E240" s="6">
         <f t="shared" si="3"/>
@@ -7369,13 +7389,13 @@
         <v>240</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="D241" s="3" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="E241" s="6">
         <f t="shared" si="3"/>
@@ -7388,13 +7408,13 @@
     <row r="242" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="1"/>
       <c r="B242" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C242" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C242" s="2" t="s">
+      <c r="D242" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="D242" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="E242" s="6">
         <f t="shared" si="3"/>
@@ -7410,13 +7430,13 @@
     <row r="243" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="1"/>
       <c r="B243" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C243" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="C243" s="2" t="s">
+      <c r="D243" s="3" t="s">
         <v>337</v>
-      </c>
-      <c r="D243" s="3" t="s">
-        <v>338</v>
       </c>
       <c r="E243" s="6">
         <f t="shared" si="3"/>

</xml_diff>